<commit_message>
Columns in node_stats_for_simulation.xlsx consistent
</commit_message>
<xml_diff>
--- a/node_stats_for_simulation.xlsx
+++ b/node_stats_for_simulation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="16160" windowHeight="10230"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="16160" windowHeight="10230" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="1651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="1650">
   <si>
     <t>nm_short</t>
   </si>
@@ -4694,9 +4694,6 @@
   </si>
   <si>
     <t>SGB</t>
-  </si>
-  <si>
-    <t>beta</t>
   </si>
   <si>
     <t>Insurance Companies</t>
@@ -5319,8 +5316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7222,9 +7219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -9656,10 +9651,10 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B122" t="s">
         <v>1561</v>
-      </c>
-      <c r="B122" t="s">
-        <v>1562</v>
       </c>
       <c r="C122">
         <v>0.13363284615384619</v>
@@ -22988,12 +22983,15 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -23010,15 +23008,15 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>1556</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="B2">
         <v>7299272.4119999995</v>
@@ -23032,13 +23030,13 @@
       <c r="F2">
         <v>5.5835108370374774E-3</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <v>1360298.3120000018</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B3">
         <v>995936</v>
@@ -23052,13 +23050,13 @@
       <c r="F3">
         <v>3.3222316368402591E-3</v>
       </c>
-      <c r="H3">
+      <c r="G3">
         <v>571035</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B4">
         <v>5319458.0000000009</v>
@@ -23072,13 +23070,13 @@
       <c r="F4">
         <v>1.72832610673418E-2</v>
       </c>
-      <c r="H4">
+      <c r="G4">
         <v>360166.00000000652</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B5">
         <v>5319458.0000000009</v>
@@ -23092,7 +23090,7 @@
       <c r="F5">
         <v>1.72832610673418E-2</v>
       </c>
-      <c r="H5">
+      <c r="G5">
         <v>360166.00000000652</v>
       </c>
     </row>
@@ -23107,7 +23105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -23139,10 +23139,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="B2" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C2">
         <v>6.4733738461538468E-3</v>
@@ -23159,10 +23159,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="B3" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C3">
         <v>2.9601569230769233E-3</v>
@@ -23179,10 +23179,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B4" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C4">
         <v>2.6969015384615395E-3</v>
@@ -23199,10 +23199,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="B5" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C5">
         <v>4.8778415384615383E-3</v>
@@ -23219,10 +23219,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B6" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="C6">
         <v>3.8947061538461545E-3</v>
@@ -23239,10 +23239,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B7" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C7">
         <v>1.7712615384615385E-3</v>
@@ -23259,10 +23259,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="B8" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C8">
         <v>6.288275384615385E-3</v>
@@ -23279,10 +23279,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B9" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C9">
         <v>1.9313452307692311E-2</v>
@@ -23299,10 +23299,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B10" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C10">
         <v>4.1792738461538456E-3</v>
@@ -23319,10 +23319,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="B11" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C11">
         <v>5.1607923076923091E-3</v>
@@ -23339,10 +23339,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="B12" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C12">
         <v>9.6019461538461529E-3</v>
@@ -23359,10 +23359,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="B13" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C13">
         <v>2.3252392307692313E-2</v>
@@ -23379,10 +23379,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="B14" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C14">
         <v>4.4887815384615374E-3</v>
@@ -23399,10 +23399,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="B15" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C15">
         <v>2.2548030769230773E-2</v>
@@ -23419,10 +23419,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="B16" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C16">
         <v>2.9211846153846151E-3</v>
@@ -23439,10 +23439,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="B17" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C17">
         <v>3.8314015384615387E-3</v>
@@ -23459,10 +23459,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B18" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C18">
         <v>1.8300876923076927E-3</v>
@@ -23479,10 +23479,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="B19" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C19">
         <v>0.29952974000000004</v>
@@ -23499,10 +23499,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="B20" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C20">
         <v>4.3576095384615356E-2</v>
@@ -23519,10 +23519,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B21" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C21">
         <v>1.0270386153846156E-2</v>
@@ -23539,10 +23539,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="B22" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C22">
         <v>3.9727730769230772E-2</v>
@@ -23559,10 +23559,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="B23" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C23">
         <v>1.1349415384615386E-3</v>
@@ -23579,10 +23579,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B24" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C24">
         <v>4.860315384615386E-3</v>
@@ -23599,10 +23599,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="B25" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C25">
         <v>3.3133553846153856E-3</v>
@@ -23619,10 +23619,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="B26" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C26">
         <v>0.1264713476923077</v>
@@ -23639,10 +23639,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B27" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C27">
         <v>3.5715846153846142E-4</v>
@@ -23659,10 +23659,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B28" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="C28">
         <v>5.2043846153846144E-4</v>
@@ -23679,10 +23679,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="B29" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C29">
         <v>7.4207713846153836E-2</v>
@@ -23699,10 +23699,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="B30" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="C30">
         <v>4.0757246153846158E-3</v>
@@ -23719,10 +23719,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="B31" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="C31">
         <v>4.4609999999999997E-3</v>
@@ -23739,10 +23739,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B32" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="C32">
         <v>7.0875815384615357E-3</v>
@@ -23759,10 +23759,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="B33" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="C33">
         <v>1.1846353846153845E-3</v>
@@ -23779,10 +23779,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="B34" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C34">
         <v>3.5063846153846143E-3</v>
@@ -23799,10 +23799,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="B35" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="C35">
         <v>3.3824507692307693E-3</v>
@@ -23819,10 +23819,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="B36" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C36">
         <v>0.14484161666666673</v>
@@ -23839,10 +23839,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="B37" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="C37">
         <v>6.6332632000000002E-2</v>
@@ -23859,10 +23859,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B38" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="C38">
         <v>0.25142443846153845</v>
@@ -23879,10 +23879,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B39" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="C39">
         <v>0.41444258923076932</v>
@@ -23899,10 +23899,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B40" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="C40">
         <v>4.2129859999999991E-2</v>
@@ -23960,10 +23960,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="B2" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C2">
         <v>2.8574846153846143E-3</v>
@@ -23980,10 +23980,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="B3" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C3">
         <v>5.0018461538461519E-3</v>
@@ -24000,10 +24000,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="B4" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C4">
         <v>6.4733738461538468E-3</v>
@@ -24020,10 +24020,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="B5" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C5">
         <v>2.9601569230769233E-3</v>
@@ -24040,10 +24040,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B6" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C6">
         <v>2.6969015384615395E-3</v>
@@ -24060,10 +24060,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="B7" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C7">
         <v>4.8778415384615383E-3</v>
@@ -24080,10 +24080,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="B8" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="C8">
         <v>7.893796923076922E-3</v>
@@ -24100,10 +24100,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B9" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="C9">
         <v>3.7162738461538457E-3</v>
@@ -24120,10 +24120,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B10" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="C10">
         <v>3.8947061538461545E-3</v>
@@ -24140,10 +24140,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B11" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="C11">
         <v>7.3687969230769208E-3</v>
@@ -24169,7 +24169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -24201,10 +24201,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B2" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C2">
         <v>1.7712615384615385E-3</v>
@@ -24221,10 +24221,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="B3" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C3">
         <v>6.288275384615385E-3</v>
@@ -24241,10 +24241,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B4" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C4">
         <v>1.9313452307692311E-2</v>
@@ -24261,10 +24261,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B5" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C5">
         <v>4.1792738461538456E-3</v>
@@ -24281,10 +24281,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="B6" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C6">
         <v>5.1607923076923091E-3</v>
@@ -24301,10 +24301,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="B7" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C7">
         <v>9.6019461538461529E-3</v>
@@ -24321,10 +24321,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="B8" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C8">
         <v>2.3252392307692313E-2</v>
@@ -24341,10 +24341,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="B9" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C9">
         <v>4.4887815384615374E-3</v>
@@ -24361,10 +24361,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="B10" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C10">
         <v>2.2548030769230773E-2</v>
@@ -24381,10 +24381,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="B11" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C11">
         <v>2.9211846153846151E-3</v>
@@ -24401,10 +24401,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="B12" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C12">
         <v>3.8314015384615387E-3</v>
@@ -24421,10 +24421,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B13" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C13">
         <v>1.8300876923076927E-3</v>
@@ -24441,10 +24441,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="B14" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C14">
         <v>0.29952974000000004</v>
@@ -24461,10 +24461,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="B15" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C15">
         <v>4.3576095384615356E-2</v>
@@ -24481,10 +24481,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B16" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C16">
         <v>1.0270386153846156E-2</v>

</xml_diff>